<commit_message>
testes -> teste de cadastro de empresas
</commit_message>
<xml_diff>
--- a/static/assets/arquivos/empresas.xlsx
+++ b/static/assets/arquivos/empresas.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\PROJETO INSS\calculadora_inss\static\assets\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D58EA6-8764-402B-9D03-B6D493983F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="0" yWindow="0" windowWidth="3804" windowHeight="2952"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -19,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>QTDD FUNC</t>
   </si>
@@ -110,13 +100,19 @@
   </si>
   <si>
     <t>Teste9</t>
+  </si>
+  <si>
+    <t>Teste10 - Gui</t>
+  </si>
+  <si>
+    <t>EmpT10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,22 +488,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.09765625" customWidth="1"/>
-    <col min="2" max="2" width="13.296875" customWidth="1"/>
-    <col min="3" max="3" width="13.59765625" customWidth="1"/>
-    <col min="4" max="5" width="13.8984375" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="5" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -524,7 +520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -541,7 +537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -558,7 +554,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -575,7 +571,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -592,7 +588,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -609,7 +605,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -626,7 +622,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -643,7 +639,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -660,7 +656,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -677,7 +673,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -694,11 +690,28 @@
         <v>24</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>45715</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" display="Emp@1"/>
-    <hyperlink ref="A5" r:id="rId2" display="Emp@1"/>
-    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId1" display="Emp@1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A5" r:id="rId2" display="Emp@1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
att: atualização de textos de erros
</commit_message>
<xml_diff>
--- a/static/assets/arquivos/empresas.xlsx
+++ b/static/assets/arquivos/empresas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
   <si>
     <t>QTDD FUNC</t>
   </si>
@@ -231,6 +231,30 @@
   </si>
   <si>
     <t>Teste32</t>
+  </si>
+  <si>
+    <t>EmpT33</t>
+  </si>
+  <si>
+    <t>EmpT34</t>
+  </si>
+  <si>
+    <t>Teste33</t>
+  </si>
+  <si>
+    <t>Teste34</t>
+  </si>
+  <si>
+    <t>EmpT35</t>
+  </si>
+  <si>
+    <t>Teste35</t>
+  </si>
+  <si>
+    <t>EmpT36</t>
+  </si>
+  <si>
+    <t>Teste36</t>
   </si>
 </sst>
 </file>
@@ -624,11 +648,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -638,7 +662,7 @@
     <col min="3" max="3" width="13.59765625" customWidth="1"/>
     <col min="4" max="4" width="22.59765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.69921875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.09765625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.59765625" bestFit="1" customWidth="1"/>
@@ -1221,6 +1245,74 @@
       </c>
       <c r="E34" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <v>45747</v>
+      </c>
+      <c r="E35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="3">
+        <v>4</v>
+      </c>
+      <c r="C36" s="3">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1">
+        <v>45747</v>
+      </c>
+      <c r="E36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="3">
+        <v>2</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2</v>
+      </c>
+      <c r="D37" s="1">
+        <v>45747</v>
+      </c>
+      <c r="E37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="3">
+        <v>3</v>
+      </c>
+      <c r="C38" s="3">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1">
+        <v>45747</v>
+      </c>
+      <c r="E38" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>